<commit_message>
Design to cost and BOM changes
</commit_message>
<xml_diff>
--- a/src/assets/BomExcel.xlsx
+++ b/src/assets/BomExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ModelMart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FileShareToMonoj\uiQA\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850BA5CC-9745-4BC8-9890-BA5993329CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA653AA7-F4E9-40E2-9E12-E5338947E644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>Comma Seperated</t>
   </si>
   <si>
-    <t>10lbs-30lbs</t>
-  </si>
-  <si>
     <t>Dash Seperated Range</t>
   </si>
   <si>
@@ -119,7 +116,10 @@
     <t>Manufacturing Location</t>
   </si>
   <si>
-    <t>China, India</t>
+    <t>10-20</t>
+  </si>
+  <si>
+    <t>China</t>
   </si>
 </sst>
 </file>
@@ -277,7 +277,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,6 +304,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -311,11 +314,6 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{17A6DD26-F95B-42C1-BE1F-2DFA767F5FD2}"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -383,6 +381,11 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -397,12 +400,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198B0C26-7FBA-4B8C-931C-7E0353545709}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198B0C26-7FBA-4B8C-931C-7E0353545709}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:C6" xr:uid="{198B0C26-7FBA-4B8C-931C-7E0353545709}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FD94368F-AA01-4A3F-9616-F18812F0FE52}" name="Engineering" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{E8E7248F-347E-4556-B5F5-753F0A57B944}" name="Input Example" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{59359431-E7B5-498C-9419-F333B5E85738}" name="Range,Miltiple Option" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FD94368F-AA01-4A3F-9616-F18812F0FE52}" name="Engineering" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E8E7248F-347E-4556-B5F5-753F0A57B944}" name="Input Example" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{59359431-E7B5-498C-9419-F333B5E85738}" name="Range,Miltiple Option" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -674,7 +677,7 @@
   <dimension ref="A1:L799"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,21 +725,21 @@
     </row>
     <row r="3" spans="1:12" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:12" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>17</v>
@@ -744,7 +747,7 @@
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>26</v>
@@ -758,10 +761,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -3986,7 +3989,7 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <titus xmlns="http://schemas.titus.com/TitusProperties/">
-  <TitusGUID xmlns="">58299b61-9dc5-4dde-99a4-00fdc6b85e1c</TitusGUID>
+  <TitusGUID xmlns="">6ae3d6e1-713e-4483-af70-1225dfc9b13c</TitusGUID>
   <TitusMetadata xmlns="">eyJucyI6Imh0dHA6XC9cL3d3dy50aXR1cy5jb21cL25zXC9UVExUSVRVUyIsInByb3BzIjpbeyJuIjoiQ2xhc3NpZmljYXRpb24iLCJ2YWxzIjpbeyJ2YWx1ZSI6IkludGVybmFsIn1dfV19</TitusMetadata>
 </titus>
 </file>

</xml_diff>